<commit_message>
finish elements and starting the functionlty
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/ecommerce.xlsx
+++ b/src/main/resources/testData/ecommerce.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="14840" firstSheet="3" activeTab="7"/>
+    <workbookView windowHeight="17160" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="newUsers" sheetId="3" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="contactUs" sheetId="7" r:id="rId6"/>
     <sheet name="searchKeywords" sheetId="10" r:id="rId7"/>
     <sheet name="dresses" sheetId="11" r:id="rId8"/>
+    <sheet name="ProductPage" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="396">
   <si>
     <t>title</t>
   </si>
@@ -1190,6 +1191,33 @@
   <si>
     <t>casual dresses,evening dresses, summer dresses</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>itemPrice</t>
+  </si>
+  <si>
+    <t>Printed Summer Dress</t>
+  </si>
+  <si>
+    <t>demo_5</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Long printed dress with thin adjustable straps. V-neckline and wiring under the bust with ruffles at the bottom of the dress.</t>
+  </si>
 </sst>
 </file>
 
@@ -1197,15 +1225,29 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="d\-mm\-yyyy"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF3A3939"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF666666"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1235,13 +1277,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -1251,14 +1286,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1272,6 +1322,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -1279,9 +1337,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1295,9 +1353,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1317,51 +1404,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1372,13 +1414,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1390,25 +1438,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1426,7 +1474,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1438,121 +1588,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1620,15 +1662,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1646,10 +1679,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1663,164 +1694,184 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="43">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1829,13 +1880,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="43" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="48" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1856,39 +1904,39 @@
     <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
     <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
-    <cellStyle name="Bad" xfId="22" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
-    <cellStyle name="Total" xfId="24" builtinId="25"/>
-    <cellStyle name="Output" xfId="25" builtinId="21"/>
-    <cellStyle name="Currency" xfId="26" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
-    <cellStyle name="Note" xfId="28" builtinId="10"/>
-    <cellStyle name="Input" xfId="29" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
-    <cellStyle name="Good" xfId="32" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="Title" xfId="38" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
-    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
-    <cellStyle name="Link" xfId="43" builtinId="8"/>
-    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
-    <cellStyle name="Comma" xfId="45" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2155,7 +2203,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:V50"/>
   <sheetViews>
@@ -2260,13 +2308,13 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="9">
         <v>18395</v>
       </c>
       <c r="G2" t="s">
@@ -2293,7 +2341,7 @@
       <c r="N2" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="3">
         <v>12345</v>
       </c>
       <c r="P2" t="s">
@@ -2328,13 +2376,13 @@
       <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="8" t="s">
         <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="9">
         <v>18396</v>
       </c>
       <c r="G3" t="s">
@@ -2361,7 +2409,7 @@
       <c r="N3" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="3">
         <v>12346</v>
       </c>
       <c r="P3" t="s">
@@ -2396,13 +2444,13 @@
       <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>52</v>
       </c>
       <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="9">
         <v>18397</v>
       </c>
       <c r="G4" t="s">
@@ -2429,7 +2477,7 @@
       <c r="N4" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="3">
         <v>12347</v>
       </c>
       <c r="P4" t="s">
@@ -2464,13 +2512,13 @@
       <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="8" t="s">
         <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="9">
         <v>18398</v>
       </c>
       <c r="G5" t="s">
@@ -2497,7 +2545,7 @@
       <c r="N5" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="3">
         <v>12348</v>
       </c>
       <c r="P5" t="s">
@@ -2532,13 +2580,13 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>71</v>
       </c>
       <c r="E6" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="9">
         <v>18399</v>
       </c>
       <c r="G6" t="s">
@@ -2565,7 +2613,7 @@
       <c r="N6" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="3">
         <v>12349</v>
       </c>
       <c r="P6" t="s">
@@ -2600,13 +2648,13 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="8" t="s">
         <v>79</v>
       </c>
       <c r="E7" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="9">
         <v>18400</v>
       </c>
       <c r="G7" t="s">
@@ -2633,7 +2681,7 @@
       <c r="N7" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="3">
         <v>12350</v>
       </c>
       <c r="P7" t="s">
@@ -2668,13 +2716,13 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>85</v>
       </c>
       <c r="E8" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="9">
         <v>18401</v>
       </c>
       <c r="G8" t="s">
@@ -2701,7 +2749,7 @@
       <c r="N8" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="3">
         <v>12351</v>
       </c>
       <c r="P8" t="s">
@@ -2736,13 +2784,13 @@
       <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="8" t="s">
         <v>91</v>
       </c>
       <c r="E9" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="9">
         <v>18402</v>
       </c>
       <c r="G9" t="s">
@@ -2769,7 +2817,7 @@
       <c r="N9" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="3">
         <v>12352</v>
       </c>
       <c r="P9" t="s">
@@ -2804,13 +2852,13 @@
       <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>97</v>
       </c>
       <c r="E10" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="9">
         <v>18403</v>
       </c>
       <c r="G10" t="s">
@@ -2837,7 +2885,7 @@
       <c r="N10" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="3">
         <v>12353</v>
       </c>
       <c r="P10" t="s">
@@ -2872,13 +2920,13 @@
       <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="8" t="s">
         <v>103</v>
       </c>
       <c r="E11" t="s">
         <v>104</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="9">
         <v>18404</v>
       </c>
       <c r="G11" t="s">
@@ -2905,7 +2953,7 @@
       <c r="N11" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O11" s="3">
         <v>12354</v>
       </c>
       <c r="P11" t="s">
@@ -2940,13 +2988,13 @@
       <c r="C12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="8" t="s">
         <v>109</v>
       </c>
       <c r="E12" t="s">
         <v>110</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="9">
         <v>18405</v>
       </c>
       <c r="G12" t="s">
@@ -2973,7 +3021,7 @@
       <c r="N12" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="3">
         <v>12355</v>
       </c>
       <c r="P12" t="s">
@@ -3008,13 +3056,13 @@
       <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="8" t="s">
         <v>115</v>
       </c>
       <c r="E13" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="9">
         <v>18406</v>
       </c>
       <c r="G13" t="s">
@@ -3041,7 +3089,7 @@
       <c r="N13" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="3">
         <v>12356</v>
       </c>
       <c r="P13" t="s">
@@ -3076,13 +3124,13 @@
       <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="5" t="s">
         <v>121</v>
       </c>
       <c r="E14" t="s">
         <v>122</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="9">
         <v>18407</v>
       </c>
       <c r="G14" t="s">
@@ -3109,7 +3157,7 @@
       <c r="N14" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="3">
         <v>12357</v>
       </c>
       <c r="P14" t="s">
@@ -3144,13 +3192,13 @@
       <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E15" t="s">
         <v>128</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="9">
         <v>18408</v>
       </c>
       <c r="G15" t="s">
@@ -3177,7 +3225,7 @@
       <c r="N15" t="s">
         <v>33</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="3">
         <v>12358</v>
       </c>
       <c r="P15" t="s">
@@ -3212,13 +3260,13 @@
       <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="8" t="s">
         <v>133</v>
       </c>
       <c r="E16" t="s">
         <v>134</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="9">
         <v>18409</v>
       </c>
       <c r="G16" t="s">
@@ -3245,7 +3293,7 @@
       <c r="N16" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="3">
         <v>12359</v>
       </c>
       <c r="P16" t="s">
@@ -3280,13 +3328,13 @@
       <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="8" t="s">
         <v>139</v>
       </c>
       <c r="E17" t="s">
         <v>140</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="9">
         <v>18410</v>
       </c>
       <c r="G17" t="s">
@@ -3313,7 +3361,7 @@
       <c r="N17" t="s">
         <v>33</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="3">
         <v>12360</v>
       </c>
       <c r="P17" t="s">
@@ -3348,13 +3396,13 @@
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="5" t="s">
         <v>145</v>
       </c>
       <c r="E18" t="s">
         <v>146</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="9">
         <v>18411</v>
       </c>
       <c r="G18" t="s">
@@ -3381,7 +3429,7 @@
       <c r="N18" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O18" s="3">
         <v>12361</v>
       </c>
       <c r="P18" t="s">
@@ -3416,13 +3464,13 @@
       <c r="C19" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="8" t="s">
         <v>151</v>
       </c>
       <c r="E19" t="s">
         <v>152</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="9">
         <v>18412</v>
       </c>
       <c r="G19" t="s">
@@ -3449,7 +3497,7 @@
       <c r="N19" t="s">
         <v>33</v>
       </c>
-      <c r="O19" s="7">
+      <c r="O19" s="3">
         <v>12362</v>
       </c>
       <c r="P19" t="s">
@@ -3484,13 +3532,13 @@
       <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="8" t="s">
         <v>157</v>
       </c>
       <c r="E20" t="s">
         <v>158</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="9">
         <v>18413</v>
       </c>
       <c r="G20" t="s">
@@ -3517,7 +3565,7 @@
       <c r="N20" t="s">
         <v>33</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="3">
         <v>12363</v>
       </c>
       <c r="P20" t="s">
@@ -3552,13 +3600,13 @@
       <c r="C21" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="8" t="s">
         <v>163</v>
       </c>
       <c r="E21" t="s">
         <v>164</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="9">
         <v>18414</v>
       </c>
       <c r="G21" t="s">
@@ -3585,7 +3633,7 @@
       <c r="N21" t="s">
         <v>33</v>
       </c>
-      <c r="O21" s="7">
+      <c r="O21" s="3">
         <v>12364</v>
       </c>
       <c r="P21" t="s">
@@ -3620,13 +3668,13 @@
       <c r="C22" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="5" t="s">
         <v>169</v>
       </c>
       <c r="E22" t="s">
         <v>170</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="9">
         <v>18415</v>
       </c>
       <c r="G22" t="s">
@@ -3653,7 +3701,7 @@
       <c r="N22" t="s">
         <v>33</v>
       </c>
-      <c r="O22" s="7">
+      <c r="O22" s="3">
         <v>12365</v>
       </c>
       <c r="P22" t="s">
@@ -3688,13 +3736,13 @@
       <c r="C23" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="8" t="s">
         <v>175</v>
       </c>
       <c r="E23" t="s">
         <v>176</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="9">
         <v>18416</v>
       </c>
       <c r="G23" t="s">
@@ -3721,7 +3769,7 @@
       <c r="N23" t="s">
         <v>33</v>
       </c>
-      <c r="O23" s="7">
+      <c r="O23" s="3">
         <v>12366</v>
       </c>
       <c r="P23" t="s">
@@ -3756,13 +3804,13 @@
       <c r="C24" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="8" t="s">
         <v>181</v>
       </c>
       <c r="E24" t="s">
         <v>182</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="9">
         <v>18417</v>
       </c>
       <c r="G24" t="s">
@@ -3789,7 +3837,7 @@
       <c r="N24" t="s">
         <v>33</v>
       </c>
-      <c r="O24" s="7">
+      <c r="O24" s="3">
         <v>12367</v>
       </c>
       <c r="P24" t="s">
@@ -3824,13 +3872,13 @@
       <c r="C25" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="8" t="s">
         <v>187</v>
       </c>
       <c r="E25" t="s">
         <v>188</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="9">
         <v>18418</v>
       </c>
       <c r="G25" t="s">
@@ -3857,7 +3905,7 @@
       <c r="N25" t="s">
         <v>33</v>
       </c>
-      <c r="O25" s="7">
+      <c r="O25" s="3">
         <v>12368</v>
       </c>
       <c r="P25" t="s">
@@ -3892,13 +3940,13 @@
       <c r="C26" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="5" t="s">
         <v>193</v>
       </c>
       <c r="E26" t="s">
         <v>194</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="9">
         <v>18419</v>
       </c>
       <c r="G26" t="s">
@@ -3925,7 +3973,7 @@
       <c r="N26" t="s">
         <v>33</v>
       </c>
-      <c r="O26" s="7">
+      <c r="O26" s="3">
         <v>12369</v>
       </c>
       <c r="P26" t="s">
@@ -3960,13 +4008,13 @@
       <c r="C27" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="8" t="s">
         <v>199</v>
       </c>
       <c r="E27" t="s">
         <v>200</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="9">
         <v>18420</v>
       </c>
       <c r="G27" t="s">
@@ -3993,7 +4041,7 @@
       <c r="N27" t="s">
         <v>33</v>
       </c>
-      <c r="O27" s="7">
+      <c r="O27" s="3">
         <v>12370</v>
       </c>
       <c r="P27" t="s">
@@ -4028,13 +4076,13 @@
       <c r="C28" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="8" t="s">
         <v>205</v>
       </c>
       <c r="E28" t="s">
         <v>206</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="9">
         <v>18421</v>
       </c>
       <c r="G28" t="s">
@@ -4061,7 +4109,7 @@
       <c r="N28" t="s">
         <v>33</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O28" s="3">
         <v>12371</v>
       </c>
       <c r="P28" t="s">
@@ -4096,13 +4144,13 @@
       <c r="C29" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="8" t="s">
         <v>211</v>
       </c>
       <c r="E29" t="s">
         <v>212</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="9">
         <v>18422</v>
       </c>
       <c r="G29" t="s">
@@ -4129,7 +4177,7 @@
       <c r="N29" t="s">
         <v>33</v>
       </c>
-      <c r="O29" s="7">
+      <c r="O29" s="3">
         <v>12372</v>
       </c>
       <c r="P29" t="s">
@@ -4164,13 +4212,13 @@
       <c r="C30" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="5" t="s">
         <v>217</v>
       </c>
       <c r="E30" t="s">
         <v>218</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="9">
         <v>18423</v>
       </c>
       <c r="G30" t="s">
@@ -4197,7 +4245,7 @@
       <c r="N30" t="s">
         <v>33</v>
       </c>
-      <c r="O30" s="7">
+      <c r="O30" s="3">
         <v>12373</v>
       </c>
       <c r="P30" t="s">
@@ -4232,13 +4280,13 @@
       <c r="C31" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="8" t="s">
         <v>223</v>
       </c>
       <c r="E31" t="s">
         <v>224</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="9">
         <v>18424</v>
       </c>
       <c r="G31" t="s">
@@ -4265,7 +4313,7 @@
       <c r="N31" t="s">
         <v>33</v>
       </c>
-      <c r="O31" s="7">
+      <c r="O31" s="3">
         <v>12374</v>
       </c>
       <c r="P31" t="s">
@@ -4300,13 +4348,13 @@
       <c r="C32" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="8" t="s">
         <v>229</v>
       </c>
       <c r="E32" t="s">
         <v>230</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="9">
         <v>18425</v>
       </c>
       <c r="G32" t="s">
@@ -4333,7 +4381,7 @@
       <c r="N32" t="s">
         <v>33</v>
       </c>
-      <c r="O32" s="7">
+      <c r="O32" s="3">
         <v>12375</v>
       </c>
       <c r="P32" t="s">
@@ -4368,13 +4416,13 @@
       <c r="C33" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="8" t="s">
         <v>235</v>
       </c>
       <c r="E33" t="s">
         <v>236</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="9">
         <v>18426</v>
       </c>
       <c r="G33" t="s">
@@ -4401,7 +4449,7 @@
       <c r="N33" t="s">
         <v>33</v>
       </c>
-      <c r="O33" s="7">
+      <c r="O33" s="3">
         <v>12376</v>
       </c>
       <c r="P33" t="s">
@@ -4436,13 +4484,13 @@
       <c r="C34" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="5" t="s">
         <v>241</v>
       </c>
       <c r="E34" t="s">
         <v>242</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="9">
         <v>18427</v>
       </c>
       <c r="G34" t="s">
@@ -4469,7 +4517,7 @@
       <c r="N34" t="s">
         <v>33</v>
       </c>
-      <c r="O34" s="7">
+      <c r="O34" s="3">
         <v>12377</v>
       </c>
       <c r="P34" t="s">
@@ -4504,13 +4552,13 @@
       <c r="C35" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="8" t="s">
         <v>247</v>
       </c>
       <c r="E35" t="s">
         <v>248</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="9">
         <v>18428</v>
       </c>
       <c r="G35" t="s">
@@ -4537,7 +4585,7 @@
       <c r="N35" t="s">
         <v>33</v>
       </c>
-      <c r="O35" s="7">
+      <c r="O35" s="3">
         <v>12378</v>
       </c>
       <c r="P35" t="s">
@@ -4572,13 +4620,13 @@
       <c r="C36" t="s">
         <v>24</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="8" t="s">
         <v>253</v>
       </c>
       <c r="E36" t="s">
         <v>254</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="9">
         <v>18429</v>
       </c>
       <c r="G36" t="s">
@@ -4605,7 +4653,7 @@
       <c r="N36" t="s">
         <v>33</v>
       </c>
-      <c r="O36" s="7">
+      <c r="O36" s="3">
         <v>12379</v>
       </c>
       <c r="P36" t="s">
@@ -4640,13 +4688,13 @@
       <c r="C37" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="8" t="s">
         <v>259</v>
       </c>
       <c r="E37" t="s">
         <v>260</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="9">
         <v>18430</v>
       </c>
       <c r="G37" t="s">
@@ -4673,7 +4721,7 @@
       <c r="N37" t="s">
         <v>33</v>
       </c>
-      <c r="O37" s="7">
+      <c r="O37" s="3">
         <v>12380</v>
       </c>
       <c r="P37" t="s">
@@ -4708,13 +4756,13 @@
       <c r="C38" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D38" s="5" t="s">
         <v>265</v>
       </c>
       <c r="E38" t="s">
         <v>266</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="9">
         <v>18431</v>
       </c>
       <c r="G38" t="s">
@@ -4741,7 +4789,7 @@
       <c r="N38" t="s">
         <v>33</v>
       </c>
-      <c r="O38" s="7">
+      <c r="O38" s="3">
         <v>12381</v>
       </c>
       <c r="P38" t="s">
@@ -4776,13 +4824,13 @@
       <c r="C39" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="8" t="s">
         <v>271</v>
       </c>
       <c r="E39" t="s">
         <v>272</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="9">
         <v>18432</v>
       </c>
       <c r="G39" t="s">
@@ -4809,7 +4857,7 @@
       <c r="N39" t="s">
         <v>33</v>
       </c>
-      <c r="O39" s="7">
+      <c r="O39" s="3">
         <v>12382</v>
       </c>
       <c r="P39" t="s">
@@ -4844,13 +4892,13 @@
       <c r="C40" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="8" t="s">
         <v>277</v>
       </c>
       <c r="E40" t="s">
         <v>278</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="9">
         <v>18433</v>
       </c>
       <c r="G40" t="s">
@@ -4877,7 +4925,7 @@
       <c r="N40" t="s">
         <v>33</v>
       </c>
-      <c r="O40" s="7">
+      <c r="O40" s="3">
         <v>12383</v>
       </c>
       <c r="P40" t="s">
@@ -4912,13 +4960,13 @@
       <c r="C41" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="8" t="s">
         <v>283</v>
       </c>
       <c r="E41" t="s">
         <v>284</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="9">
         <v>18434</v>
       </c>
       <c r="G41" t="s">
@@ -4945,7 +4993,7 @@
       <c r="N41" t="s">
         <v>33</v>
       </c>
-      <c r="O41" s="7">
+      <c r="O41" s="3">
         <v>12384</v>
       </c>
       <c r="P41" t="s">
@@ -4980,13 +5028,13 @@
       <c r="C42" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="5" t="s">
         <v>289</v>
       </c>
       <c r="E42" t="s">
         <v>290</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="9">
         <v>18435</v>
       </c>
       <c r="G42" t="s">
@@ -5013,7 +5061,7 @@
       <c r="N42" t="s">
         <v>33</v>
       </c>
-      <c r="O42" s="7">
+      <c r="O42" s="3">
         <v>12385</v>
       </c>
       <c r="P42" t="s">
@@ -5048,13 +5096,13 @@
       <c r="C43" t="s">
         <v>24</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="8" t="s">
         <v>295</v>
       </c>
       <c r="E43" t="s">
         <v>296</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="9">
         <v>18436</v>
       </c>
       <c r="G43" t="s">
@@ -5081,7 +5129,7 @@
       <c r="N43" t="s">
         <v>33</v>
       </c>
-      <c r="O43" s="7">
+      <c r="O43" s="3">
         <v>12386</v>
       </c>
       <c r="P43" t="s">
@@ -5116,13 +5164,13 @@
       <c r="C44" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="8" t="s">
         <v>301</v>
       </c>
       <c r="E44" t="s">
         <v>302</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="9">
         <v>18437</v>
       </c>
       <c r="G44" t="s">
@@ -5149,7 +5197,7 @@
       <c r="N44" t="s">
         <v>33</v>
       </c>
-      <c r="O44" s="7">
+      <c r="O44" s="3">
         <v>12387</v>
       </c>
       <c r="P44" t="s">
@@ -5184,13 +5232,13 @@
       <c r="C45" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="8" t="s">
         <v>307</v>
       </c>
       <c r="E45" t="s">
         <v>308</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="9">
         <v>18438</v>
       </c>
       <c r="G45" t="s">
@@ -5217,7 +5265,7 @@
       <c r="N45" t="s">
         <v>33</v>
       </c>
-      <c r="O45" s="7">
+      <c r="O45" s="3">
         <v>12388</v>
       </c>
       <c r="P45" t="s">
@@ -5252,13 +5300,13 @@
       <c r="C46" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="5" t="s">
         <v>313</v>
       </c>
       <c r="E46" t="s">
         <v>314</v>
       </c>
-      <c r="F46" s="6">
+      <c r="F46" s="9">
         <v>18439</v>
       </c>
       <c r="G46" t="s">
@@ -5285,7 +5333,7 @@
       <c r="N46" t="s">
         <v>33</v>
       </c>
-      <c r="O46" s="7">
+      <c r="O46" s="3">
         <v>12389</v>
       </c>
       <c r="P46" t="s">
@@ -5320,13 +5368,13 @@
       <c r="C47" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="8" t="s">
         <v>319</v>
       </c>
       <c r="E47" t="s">
         <v>320</v>
       </c>
-      <c r="F47" s="6">
+      <c r="F47" s="9">
         <v>18440</v>
       </c>
       <c r="G47" t="s">
@@ -5353,7 +5401,7 @@
       <c r="N47" t="s">
         <v>33</v>
       </c>
-      <c r="O47" s="7">
+      <c r="O47" s="3">
         <v>12390</v>
       </c>
       <c r="P47" t="s">
@@ -5388,13 +5436,13 @@
       <c r="C48" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="8" t="s">
         <v>325</v>
       </c>
       <c r="E48" t="s">
         <v>326</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="9">
         <v>18441</v>
       </c>
       <c r="G48" t="s">
@@ -5421,7 +5469,7 @@
       <c r="N48" t="s">
         <v>33</v>
       </c>
-      <c r="O48" s="7">
+      <c r="O48" s="3">
         <v>12391</v>
       </c>
       <c r="P48" t="s">
@@ -5456,13 +5504,13 @@
       <c r="C49" t="s">
         <v>24</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="8" t="s">
         <v>331</v>
       </c>
       <c r="E49" t="s">
         <v>332</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49" s="9">
         <v>18442</v>
       </c>
       <c r="G49" t="s">
@@ -5489,7 +5537,7 @@
       <c r="N49" t="s">
         <v>33</v>
       </c>
-      <c r="O49" s="7">
+      <c r="O49" s="3">
         <v>12392</v>
       </c>
       <c r="P49" t="s">
@@ -5524,13 +5572,13 @@
       <c r="C50" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="5" t="s">
         <v>337</v>
       </c>
       <c r="E50" t="s">
         <v>338</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F50" s="9">
         <v>18443</v>
       </c>
       <c r="G50" t="s">
@@ -5557,7 +5605,7 @@
       <c r="N50" t="s">
         <v>33</v>
       </c>
-      <c r="O50" s="7">
+      <c r="O50" s="3">
         <v>12393</v>
       </c>
       <c r="P50" t="s">
@@ -5640,7 +5688,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -5662,7 +5710,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>343</v>
       </c>
       <c r="B2" t="s">
@@ -5679,7 +5727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -5702,7 +5750,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>346</v>
       </c>
       <c r="B2" t="s">
@@ -5710,15 +5758,15 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>349</v>
       </c>
       <c r="B4" t="s">
@@ -5737,7 +5785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -5764,7 +5812,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>343</v>
       </c>
       <c r="B2" t="s">
@@ -5794,7 +5842,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>343</v>
       </c>
       <c r="C5" t="s">
@@ -5812,7 +5860,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -5831,7 +5879,7 @@
       </c>
     </row>
     <row r="2" ht="126" spans="1:1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>355</v>
       </c>
     </row>
@@ -5842,7 +5890,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -5883,7 +5931,7 @@
       <c r="A2" t="s">
         <v>362</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>363</v>
       </c>
       <c r="C2" t="s">
@@ -5903,7 +5951,7 @@
       <c r="A3" t="s">
         <v>367</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>368</v>
       </c>
       <c r="C3" t="s">
@@ -5923,7 +5971,7 @@
       <c r="A4" t="s">
         <v>362</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>343</v>
       </c>
       <c r="D4" t="s">
@@ -5948,7 +5996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -5981,7 +6029,7 @@
       <c r="B2" t="s">
         <v>376</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>377</v>
       </c>
     </row>
@@ -5992,7 +6040,7 @@
       <c r="B3" t="s">
         <v>376</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>377</v>
       </c>
     </row>
@@ -6003,7 +6051,7 @@
       <c r="B4" t="s">
         <v>380</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>377</v>
       </c>
     </row>
@@ -6014,7 +6062,7 @@
       <c r="B5" t="s">
         <v>380</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>377</v>
       </c>
     </row>
@@ -6025,12 +6073,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -6062,4 +6110,59 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="28.390625" customWidth="1"/>
+    <col min="4" max="4" width="92.0546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="2" ht="19" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C2" t="s">
+        <v>394</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E2" s="3">
+        <v>28.98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add to cart finished
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/ecommerce.xlsx
+++ b/src/main/resources/testData/ecommerce.xlsx
@@ -22,14 +22,14 @@
     <sheet name="contactUs" sheetId="7" r:id="rId7"/>
     <sheet name="searchKeywords" sheetId="8" r:id="rId8"/>
     <sheet name="dresses" sheetId="9" r:id="rId9"/>
-    <sheet name="ProductPage" sheetId="10" r:id="rId10"/>
+    <sheet name="ProductPage" sheetId="11" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -124,15 +124,7 @@
     <t>Peterson</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson12@abc.com</t>
-    </r>
+    <t>sandy.peterson12@abc.com</t>
   </si>
   <si>
     <t>S-12Peter!</t>
@@ -180,15 +172,7 @@
     <t>Sam</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson13@abc.com</t>
-    </r>
+    <t>sam.peterson13@abc.com</t>
   </si>
   <si>
     <t>S-13Peter!</t>
@@ -221,15 +205,7 @@
     <t>Hillary</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson14@abc.com</t>
-    </r>
+    <t>hillary.peterson14@abc.com</t>
   </si>
   <si>
     <t>S-14Peter!</t>
@@ -259,15 +235,7 @@
     <t>Michael</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson15@abc.com</t>
-    </r>
+    <t>michael.peterson15@abc.com</t>
   </si>
   <si>
     <t>S-15Peter!</t>
@@ -294,15 +262,7 @@
     <t>800-666-6669</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson13@abc.com</t>
-    </r>
+    <t>sandy.peterson13@abc.com</t>
   </si>
   <si>
     <t>S-16Peter!</t>
@@ -326,15 +286,7 @@
     <t>800-666-6670</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson14@abc.com</t>
-    </r>
+    <t>sam.peterson14@abc.com</t>
   </si>
   <si>
     <t>S-17Peter!</t>
@@ -352,15 +304,7 @@
     <t>800-666-6671</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson15@abc.com</t>
-    </r>
+    <t>hillary.peterson15@abc.com</t>
   </si>
   <si>
     <t>S-18Peter!</t>
@@ -378,15 +322,7 @@
     <t>800-666-6672</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson16@abc.com</t>
-    </r>
+    <t>michael.peterson16@abc.com</t>
   </si>
   <si>
     <t>S-19Peter!</t>
@@ -404,15 +340,7 @@
     <t>800-666-6673</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson14@abc.com</t>
-    </r>
+    <t>sandy.peterson14@abc.com</t>
   </si>
   <si>
     <t>S-20Peter!</t>
@@ -430,15 +358,7 @@
     <t>800-666-6674</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson15@abc.com</t>
-    </r>
+    <t>sam.peterson15@abc.com</t>
   </si>
   <si>
     <t>S-21Peter!</t>
@@ -456,15 +376,7 @@
     <t>800-666-6675</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson16@abc.com</t>
-    </r>
+    <t>hillary.peterson16@abc.com</t>
   </si>
   <si>
     <t>S-22Peter!</t>
@@ -482,15 +394,7 @@
     <t>800-666-6676</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson17@abc.com</t>
-    </r>
+    <t>michael.peterson17@abc.com</t>
   </si>
   <si>
     <t>S-23Peter!</t>
@@ -508,15 +412,7 @@
     <t>800-666-6677</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson15@abc.com</t>
-    </r>
+    <t>sandy.peterson15@abc.com</t>
   </si>
   <si>
     <t>S-24Peter!</t>
@@ -534,15 +430,7 @@
     <t>800-666-6678</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson16@abc.com</t>
-    </r>
+    <t>sam.peterson16@abc.com</t>
   </si>
   <si>
     <t>S-25Peter!</t>
@@ -560,15 +448,7 @@
     <t>800-666-6679</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson17@abc.com</t>
-    </r>
+    <t>hillary.peterson17@abc.com</t>
   </si>
   <si>
     <t>S-26Peter!</t>
@@ -586,15 +466,7 @@
     <t>800-666-6680</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson18@abc.com</t>
-    </r>
+    <t>michael.peterson18@abc.com</t>
   </si>
   <si>
     <t>S-27Peter!</t>
@@ -612,15 +484,7 @@
     <t>800-666-6681</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson16@abc.com</t>
-    </r>
+    <t>sandy.peterson16@abc.com</t>
   </si>
   <si>
     <t>S-28Peter!</t>
@@ -638,15 +502,7 @@
     <t>800-666-6682</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson17@abc.com</t>
-    </r>
+    <t>sam.peterson17@abc.com</t>
   </si>
   <si>
     <t>S-29Peter!</t>
@@ -664,15 +520,7 @@
     <t>800-666-6683</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson18@abc.com</t>
-    </r>
+    <t>hillary.peterson18@abc.com</t>
   </si>
   <si>
     <t>S-30Peter!</t>
@@ -690,15 +538,7 @@
     <t>800-666-6684</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson19@abc.com</t>
-    </r>
+    <t>michael.peterson19@abc.com</t>
   </si>
   <si>
     <t>S-31Peter!</t>
@@ -716,15 +556,7 @@
     <t>800-666-6685</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson17@abc.com</t>
-    </r>
+    <t>sandy.peterson17@abc.com</t>
   </si>
   <si>
     <t>S-32Peter!</t>
@@ -742,15 +574,7 @@
     <t>800-666-6686</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson18@abc.com</t>
-    </r>
+    <t>sam.peterson18@abc.com</t>
   </si>
   <si>
     <t>S-33Peter!</t>
@@ -768,15 +592,7 @@
     <t>800-666-6687</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson19@abc.com</t>
-    </r>
+    <t>hillary.peterson19@abc.com</t>
   </si>
   <si>
     <t>S-34Peter!</t>
@@ -794,15 +610,7 @@
     <t>800-666-6688</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson20@abc.com</t>
-    </r>
+    <t>michael.peterson20@abc.com</t>
   </si>
   <si>
     <t>S-35Peter!</t>
@@ -820,15 +628,7 @@
     <t>800-666-6689</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson18@abc.com</t>
-    </r>
+    <t>sandy.peterson18@abc.com</t>
   </si>
   <si>
     <t>S-36Peter!</t>
@@ -846,15 +646,7 @@
     <t>800-666-6690</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson19@abc.com</t>
-    </r>
+    <t>sam.peterson19@abc.com</t>
   </si>
   <si>
     <t>S-37Peter!</t>
@@ -872,15 +664,7 @@
     <t>800-666-6691</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson20@abc.com</t>
-    </r>
+    <t>hillary.peterson20@abc.com</t>
   </si>
   <si>
     <t>S-38Peter!</t>
@@ -898,15 +682,7 @@
     <t>800-666-6692</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson21@abc.com</t>
-    </r>
+    <t>michael.peterson21@abc.com</t>
   </si>
   <si>
     <t>S-39Peter!</t>
@@ -924,15 +700,7 @@
     <t>800-666-6693</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson19@abc.com</t>
-    </r>
+    <t>sandy.peterson19@abc.com</t>
   </si>
   <si>
     <t>S-40Peter!</t>
@@ -950,15 +718,7 @@
     <t>800-666-6694</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson20@abc.com</t>
-    </r>
+    <t>sam.peterson20@abc.com</t>
   </si>
   <si>
     <t>S-41Peter!</t>
@@ -976,15 +736,7 @@
     <t>800-666-6695</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson21@abc.com</t>
-    </r>
+    <t>hillary.peterson21@abc.com</t>
   </si>
   <si>
     <t>S-42Peter!</t>
@@ -1002,15 +754,7 @@
     <t>800-666-6696</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson22@abc.com</t>
-    </r>
+    <t>michael.peterson22@abc.com</t>
   </si>
   <si>
     <t>S-43Peter!</t>
@@ -1028,15 +772,7 @@
     <t>800-666-6697</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson20@abc.com</t>
-    </r>
+    <t>sandy.peterson20@abc.com</t>
   </si>
   <si>
     <t>S-44Peter!</t>
@@ -1054,15 +790,7 @@
     <t>800-666-6698</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson21@abc.com</t>
-    </r>
+    <t>sam.peterson21@abc.com</t>
   </si>
   <si>
     <t>S-45Peter!</t>
@@ -1080,15 +808,7 @@
     <t>800-666-6699</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson22@abc.com</t>
-    </r>
+    <t>hillary.peterson22@abc.com</t>
   </si>
   <si>
     <t>S-46Peter!</t>
@@ -1106,15 +826,7 @@
     <t>800-666-6700</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson23@abc.com</t>
-    </r>
+    <t>michael.peterson23@abc.com</t>
   </si>
   <si>
     <t>S-47Peter!</t>
@@ -1132,15 +844,7 @@
     <t>800-666-6701</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson21@abc.com</t>
-    </r>
+    <t>sandy.peterson21@abc.com</t>
   </si>
   <si>
     <t>S-48Peter!</t>
@@ -1158,15 +862,7 @@
     <t>800-666-6702</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson22@abc.com</t>
-    </r>
+    <t>sam.peterson22@abc.com</t>
   </si>
   <si>
     <t>S-49Peter!</t>
@@ -1184,15 +880,7 @@
     <t>800-666-6703</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson23@abc.com</t>
-    </r>
+    <t>hillary.peterson23@abc.com</t>
   </si>
   <si>
     <t>S-50Peter!</t>
@@ -1210,15 +898,7 @@
     <t>800-666-6704</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson24@abc.com</t>
-    </r>
+    <t>michael.peterson24@abc.com</t>
   </si>
   <si>
     <t>S-51Peter!</t>
@@ -1236,15 +916,7 @@
     <t>800-666-6705</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson22@abc.com</t>
-    </r>
+    <t>sandy.peterson22@abc.com</t>
   </si>
   <si>
     <t>S-52Peter!</t>
@@ -1262,15 +934,7 @@
     <t>800-666-6706</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson23@abc.com</t>
-    </r>
+    <t>sam.peterson23@abc.com</t>
   </si>
   <si>
     <t>S-53Peter!</t>
@@ -1288,15 +952,7 @@
     <t>800-666-6707</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson24@abc.com</t>
-    </r>
+    <t>hillary.peterson24@abc.com</t>
   </si>
   <si>
     <t>S-54Peter!</t>
@@ -1314,15 +970,7 @@
     <t>800-666-6708</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson25@abc.com</t>
-    </r>
+    <t>michael.peterson25@abc.com</t>
   </si>
   <si>
     <t>S-55Peter!</t>
@@ -1340,15 +988,7 @@
     <t>800-666-6709</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson23@abc.com</t>
-    </r>
+    <t>sandy.peterson23@abc.com</t>
   </si>
   <si>
     <t>S-56Peter!</t>
@@ -1366,15 +1006,7 @@
     <t>800-666-6710</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sam.peterson24@abc.com</t>
-    </r>
+    <t>sam.peterson24@abc.com</t>
   </si>
   <si>
     <t>S-57Peter!</t>
@@ -1392,15 +1024,7 @@
     <t>800-666-6711</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>hillary.peterson25@abc.com</t>
-    </r>
+    <t>hillary.peterson25@abc.com</t>
   </si>
   <si>
     <t>S-58Peter!</t>
@@ -1418,15 +1042,7 @@
     <t>800-666-6712</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="13"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>michael.peterson26@abc.com</t>
-    </r>
+    <t>michael.peterson26@abc.com</t>
   </si>
   <si>
     <t>S-59Peter!</t>
@@ -1444,15 +1060,7 @@
     <t>800-666-6713</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>sandy.peterson24@abc.com</t>
-    </r>
+    <t>sandy.peterson24@abc.com</t>
   </si>
   <si>
     <t>S-60Peter!</t>
@@ -1473,15 +1081,7 @@
     <t>userLogin</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>kevinlee1234@gmail.com</t>
-    </r>
+    <t>kevinlee1234@gmail.com</t>
   </si>
   <si>
     <t>Kevin123</t>
@@ -1493,15 +1093,7 @@
     <t>errorMessages</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>kevinlee1234@gmail</t>
-    </r>
+    <t>kevinlee1234@gmail</t>
   </si>
   <si>
     <t>Invalid email address.</t>
@@ -1510,15 +1102,7 @@
     <t>An account using this email address has already been registered. Please enter a valid password or request a new one.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>kevinlee1234</t>
-    </r>
+    <t>kevinlee1234</t>
   </si>
   <si>
     <t>negativeLogin</t>
@@ -1576,15 +1160,7 @@
     <t>Webmaster</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>henry123@abc.com</t>
-    </r>
+    <t>henry123@abc.com</t>
   </si>
   <si>
     <t>KDF3454GH</t>
@@ -1599,15 +1175,7 @@
     <t>Customer service</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>henry124@abc.com</t>
-    </r>
+    <t>henry124@abc.com</t>
   </si>
   <si>
     <t>LPDJ4689KL</t>
@@ -1722,6 +1290,30 @@
   </si>
   <si>
     <t>Peter@gmail.com</t>
+  </si>
+  <si>
+    <t>fdtrg</t>
+  </si>
+  <si>
+    <t>PickColor</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>ShippingCost</t>
+  </si>
+  <si>
+    <t>TotalCost</t>
   </si>
 </sst>
 </file>
@@ -1731,7 +1323,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d&quot;-&quot;mm&quot;-&quot;yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1802,6 +1394,10 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1890,7 +1486,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2015,6 +1611,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="13" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3182,20 +2781,22 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="30.52734375" customWidth="1"/>
+    <col min="2" max="2" width="30.52734375" customWidth="1"/>
+    <col min="3" max="3" width="30.52734375" customWidth="1"/>
+    <col min="4" max="4" width="30.52734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" customHeight="1" ht="48">
       <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="23"/>
       <c r="D3" s="23"/>
     </row>
-    <row r="7" spans="2:4" ht="18" x14ac:dyDescent="0.5">
+    <row r="7" ht="18">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -3206,14 +2807,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="9" ht="15">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="10" ht="15">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -3222,14 +2823,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="11" ht="15">
       <c r="B11" s="2" t="s">
         <v>349</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="12" ht="15">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -3238,14 +2839,14 @@
         <v>349</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="13" ht="15">
       <c r="B13" s="2" t="s">
         <v>352</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="14" ht="15">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -3254,14 +2855,14 @@
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="15" ht="15">
       <c r="B15" s="2" t="s">
         <v>358</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="16" ht="15">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -3270,14 +2871,14 @@
         <v>358</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="17" ht="15">
       <c r="B17" s="2" t="s">
         <v>364</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="18" ht="15">
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
         <v>5</v>
@@ -3286,14 +2887,14 @@
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="19" ht="15">
       <c r="B19" s="2" t="s">
         <v>366</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="20" ht="15">
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>5</v>
@@ -3302,14 +2903,14 @@
         <v>366</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="21" ht="15">
       <c r="B21" s="2" t="s">
         <v>383</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="22" ht="15">
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -3318,14 +2919,14 @@
         <v>383</v>
       </c>
     </row>
-    <row r="23" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="23" ht="15">
       <c r="B23" s="2" t="s">
         <v>394</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="24" ht="15">
       <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
         <v>5</v>
@@ -3334,14 +2935,14 @@
         <v>394</v>
       </c>
     </row>
-    <row r="25" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="25" ht="15">
       <c r="B25" s="2" t="s">
         <v>399</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" ht="15.7" x14ac:dyDescent="0.5">
+    <row r="26" ht="15">
       <c r="B26" s="3"/>
       <c r="C26" s="3" t="s">
         <v>5</v>
@@ -3370,30 +2971,15 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:K10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="A1" activeCellId="0" sqref="1:2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="24.46875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="12.52734375" style="21" customWidth="1"/>
-    <col min="3" max="3" width="9.9375" style="21" customWidth="1"/>
-    <col min="4" max="4" width="31.3515625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="16.05859375" style="21" customWidth="1"/>
-    <col min="6" max="6" width="9" style="21" customWidth="1"/>
-    <col min="7" max="7" width="11.1171875" style="21" customWidth="1"/>
-    <col min="8" max="8" width="14.5859375" style="21" customWidth="1"/>
-    <col min="9" max="9" width="11.703125" style="21" customWidth="1"/>
-    <col min="10" max="10" width="14.05859375" style="21" customWidth="1"/>
-    <col min="11" max="11" width="15.76171875" style="21" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="21"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1">
       <c r="A1" s="31" t="s">
         <v>400</v>
       </c>
@@ -3424,11 +3010,26 @@
       <c r="J1" s="34" t="s">
         <v>410</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="34" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="L1" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" ht="18">
       <c r="A2" s="35" t="s">
         <v>405</v>
       </c>
@@ -3448,7 +3049,7 @@
         <v>30.51</v>
       </c>
       <c r="G2" s="38">
-        <v>0.05</v>
+        <v>5E-2</v>
       </c>
       <c r="H2" s="34">
         <v>4</v>
@@ -3462,120 +3063,28 @@
       <c r="K2" s="41" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="24"/>
-    </row>
-    <row r="4" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-    </row>
-    <row r="5" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-    </row>
-    <row r="6" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-    </row>
-    <row r="7" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-    </row>
-    <row r="8" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-    </row>
-    <row r="9" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-    </row>
-    <row r="10" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
+      <c r="L2" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>422</v>
+      </c>
+      <c r="N2" s="0">
+        <v>2</v>
+      </c>
+      <c r="O2" s="0">
+        <v>2</v>
+      </c>
+      <c r="P2" s="0">
+        <f>E2*N2+O2</f>
+        <v>59.96</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{961FA685-23C6-4EC9-9FAE-528022F10CC8}"/>
+    <hyperlink ref="K2" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3585,9 +3094,11 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="3" width="9" style="5" customWidth="1"/>
+    <col min="1" max="1" width="9" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9" style="5" customWidth="1"/>
     <col min="4" max="4" width="27.46875" style="5" customWidth="1"/>
     <col min="5" max="5" width="9" style="5" customWidth="1"/>
     <col min="6" max="6" width="12.46875" style="5" customWidth="1"/>
@@ -3598,7 +3109,8 @@
     <col min="11" max="11" width="9" style="5" customWidth="1"/>
     <col min="12" max="12" width="13" style="5" customWidth="1"/>
     <col min="13" max="13" width="14.64453125" style="5" customWidth="1"/>
-    <col min="14" max="15" width="12.46875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="12.46875" style="5" customWidth="1"/>
+    <col min="15" max="15" width="12.46875" style="5" customWidth="1"/>
     <col min="16" max="16" width="41.46875" style="5" customWidth="1"/>
     <col min="17" max="17" width="12.46875" style="5" customWidth="1"/>
     <col min="18" max="18" width="13.3515625" style="5" customWidth="1"/>
@@ -3610,7 +3122,7 @@
     <col min="24" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" customHeight="1" ht="15">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -3678,7 +3190,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" customHeight="1" ht="15">
       <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
@@ -3746,7 +3258,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" customHeight="1" ht="15">
       <c r="A3" s="6" t="s">
         <v>45</v>
       </c>
@@ -3814,7 +3326,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" customHeight="1" ht="15">
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
@@ -3882,7 +3394,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" customHeight="1" ht="15">
       <c r="A5" s="6" t="s">
         <v>45</v>
       </c>
@@ -3950,7 +3462,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" customHeight="1" ht="15">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -4018,7 +3530,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" customHeight="1" ht="15">
       <c r="A7" s="6" t="s">
         <v>45</v>
       </c>
@@ -4086,7 +3598,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" customHeight="1" ht="15">
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
@@ -4154,7 +3666,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" customHeight="1" ht="15">
       <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
@@ -4222,7 +3734,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" customHeight="1" ht="15">
       <c r="A10" s="6" t="s">
         <v>28</v>
       </c>
@@ -4290,7 +3802,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" customHeight="1" ht="15">
       <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
@@ -4358,7 +3870,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" customHeight="1" ht="15">
       <c r="A12" s="6" t="s">
         <v>28</v>
       </c>
@@ -4426,7 +3938,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" customHeight="1" ht="15">
       <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
@@ -4494,7 +4006,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" customHeight="1" ht="15">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -4562,7 +4074,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" customHeight="1" ht="15">
       <c r="A15" s="6" t="s">
         <v>45</v>
       </c>
@@ -4630,7 +4142,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" customHeight="1" ht="15">
       <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
@@ -4698,7 +4210,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" customHeight="1" ht="15">
       <c r="A17" s="6" t="s">
         <v>45</v>
       </c>
@@ -4766,7 +4278,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" customHeight="1" ht="15">
       <c r="A18" s="6" t="s">
         <v>28</v>
       </c>
@@ -4834,7 +4346,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" customHeight="1" ht="15">
       <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
@@ -4902,7 +4414,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" customHeight="1" ht="15">
       <c r="A20" s="6" t="s">
         <v>28</v>
       </c>
@@ -4970,7 +4482,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" customHeight="1" ht="15">
       <c r="A21" s="6" t="s">
         <v>45</v>
       </c>
@@ -5038,7 +4550,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" customHeight="1" ht="15">
       <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
@@ -5106,7 +4618,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" customHeight="1" ht="15">
       <c r="A23" s="6" t="s">
         <v>45</v>
       </c>
@@ -5174,7 +4686,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="24" customHeight="1" ht="15">
       <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
@@ -5242,7 +4754,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="25" customHeight="1" ht="15">
       <c r="A25" s="6" t="s">
         <v>45</v>
       </c>
@@ -5310,7 +4822,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="26" customHeight="1" ht="15">
       <c r="A26" s="6" t="s">
         <v>28</v>
       </c>
@@ -5378,7 +4890,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" customHeight="1" ht="15">
       <c r="A27" s="6" t="s">
         <v>45</v>
       </c>
@@ -5446,7 +4958,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="28" customHeight="1" ht="15">
       <c r="A28" s="6" t="s">
         <v>28</v>
       </c>
@@ -5514,7 +5026,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="29" customHeight="1" ht="15">
       <c r="A29" s="6" t="s">
         <v>45</v>
       </c>
@@ -5582,7 +5094,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" customHeight="1" ht="15">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -5650,7 +5162,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" customHeight="1" ht="15">
       <c r="A31" s="6" t="s">
         <v>45</v>
       </c>
@@ -5718,7 +5230,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="32" customHeight="1" ht="15">
       <c r="A32" s="6" t="s">
         <v>28</v>
       </c>
@@ -5786,7 +5298,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="33" customHeight="1" ht="15">
       <c r="A33" s="6" t="s">
         <v>45</v>
       </c>
@@ -5854,7 +5366,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="34" customHeight="1" ht="15">
       <c r="A34" s="6" t="s">
         <v>28</v>
       </c>
@@ -5922,7 +5434,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="35" customHeight="1" ht="15">
       <c r="A35" s="6" t="s">
         <v>45</v>
       </c>
@@ -5990,7 +5502,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="36" customHeight="1" ht="15">
       <c r="A36" s="6" t="s">
         <v>28</v>
       </c>
@@ -6058,7 +5570,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="37" customHeight="1" ht="15">
       <c r="A37" s="6" t="s">
         <v>45</v>
       </c>
@@ -6126,7 +5638,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="38" customHeight="1" ht="15">
       <c r="A38" s="6" t="s">
         <v>28</v>
       </c>
@@ -6194,7 +5706,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="39" customHeight="1" ht="15">
       <c r="A39" s="6" t="s">
         <v>45</v>
       </c>
@@ -6262,7 +5774,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="40" customHeight="1" ht="15">
       <c r="A40" s="6" t="s">
         <v>28</v>
       </c>
@@ -6330,7 +5842,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="41" customHeight="1" ht="15">
       <c r="A41" s="6" t="s">
         <v>45</v>
       </c>
@@ -6398,7 +5910,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="42" customHeight="1" ht="15">
       <c r="A42" s="6" t="s">
         <v>28</v>
       </c>
@@ -6466,7 +5978,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="43" customHeight="1" ht="15">
       <c r="A43" s="6" t="s">
         <v>45</v>
       </c>
@@ -6534,7 +6046,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="44" customHeight="1" ht="15">
       <c r="A44" s="6" t="s">
         <v>28</v>
       </c>
@@ -6602,7 +6114,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="45" customHeight="1" ht="15">
       <c r="A45" s="6" t="s">
         <v>45</v>
       </c>
@@ -6670,7 +6182,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="46" customHeight="1" ht="15">
       <c r="A46" s="6" t="s">
         <v>28</v>
       </c>
@@ -6738,7 +6250,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="47" customHeight="1" ht="15">
       <c r="A47" s="6" t="s">
         <v>45</v>
       </c>
@@ -6806,7 +6318,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="48" customHeight="1" ht="15">
       <c r="A48" s="6" t="s">
         <v>28</v>
       </c>
@@ -6874,7 +6386,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="49" customHeight="1" ht="15">
       <c r="A49" s="6" t="s">
         <v>45</v>
       </c>
@@ -6942,7 +6454,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="50" customHeight="1" ht="15">
       <c r="A50" s="6" t="s">
         <v>28</v>
       </c>
@@ -7076,14 +6588,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="22.46875" style="11" customWidth="1"/>
-    <col min="2" max="6" width="9" style="11" customWidth="1"/>
+    <col min="2" max="2" width="9" style="11" customWidth="1"/>
+    <col min="3" max="3" width="9" style="11" customWidth="1"/>
+    <col min="4" max="4" width="9" style="11" customWidth="1"/>
+    <col min="5" max="5" width="9" style="11" customWidth="1"/>
+    <col min="6" max="6" width="9" style="11" customWidth="1"/>
     <col min="7" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" customHeight="1" ht="15">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -7094,7 +6610,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" customHeight="1" ht="15">
       <c r="A2" s="7" t="s">
         <v>350</v>
       </c>
@@ -7105,56 +6621,56 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" customHeight="1" ht="15">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" customHeight="1" ht="15">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" customHeight="1" ht="15">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" customHeight="1" ht="15">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" customHeight="1" ht="15">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" customHeight="1" ht="15">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" customHeight="1" ht="15">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" customHeight="1" ht="15">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -7179,15 +6695,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="21" style="13" customWidth="1"/>
     <col min="2" max="2" width="19.3515625" style="13" customWidth="1"/>
-    <col min="3" max="6" width="9" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9" style="13" customWidth="1"/>
+    <col min="4" max="4" width="9" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9" style="13" customWidth="1"/>
+    <col min="6" max="6" width="9" style="13" customWidth="1"/>
     <col min="7" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" customHeight="1" ht="15">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -7198,7 +6717,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" customHeight="1" ht="15">
       <c r="A2" s="7" t="s">
         <v>354</v>
       </c>
@@ -7209,7 +6728,7 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" customHeight="1" ht="15">
       <c r="A3" s="7" t="s">
         <v>350</v>
       </c>
@@ -7220,7 +6739,7 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" customHeight="1" ht="15">
       <c r="A4" s="7" t="s">
         <v>357</v>
       </c>
@@ -7231,42 +6750,42 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" customHeight="1" ht="15">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" customHeight="1" ht="15">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" customHeight="1" ht="15">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" customHeight="1" ht="15">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" customHeight="1" ht="15">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" customHeight="1" ht="15">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -7293,16 +6812,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="21" style="14" customWidth="1"/>
     <col min="2" max="2" width="9.17578125" style="14" customWidth="1"/>
     <col min="3" max="3" width="103.17578125" style="14" customWidth="1"/>
-    <col min="4" max="6" width="9" style="14" customWidth="1"/>
+    <col min="4" max="4" width="9" style="14" customWidth="1"/>
+    <col min="5" max="5" width="9" style="14" customWidth="1"/>
+    <col min="6" max="6" width="9" style="14" customWidth="1"/>
     <col min="7" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" customHeight="1" ht="15">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -7315,7 +6836,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" customHeight="1" ht="15">
       <c r="A2" s="7" t="s">
         <v>350</v>
       </c>
@@ -7328,7 +6849,7 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" customHeight="1" ht="15">
       <c r="A3" s="6" t="s">
         <v>361</v>
       </c>
@@ -7341,7 +6862,7 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" customHeight="1" ht="15">
       <c r="A4" s="12"/>
       <c r="B4" s="6" t="s">
         <v>351</v>
@@ -7352,7 +6873,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" customHeight="1" ht="15">
       <c r="A5" s="7" t="s">
         <v>350</v>
       </c>
@@ -7363,35 +6884,35 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" customHeight="1" ht="15">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" customHeight="1" ht="15">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" customHeight="1" ht="15">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" customHeight="1" ht="15">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" customHeight="1" ht="15">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -7417,14 +6938,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="47.17578125" style="15" customWidth="1"/>
-    <col min="2" max="6" width="9" style="15" customWidth="1"/>
+    <col min="2" max="2" width="9" style="15" customWidth="1"/>
+    <col min="3" max="3" width="9" style="15" customWidth="1"/>
+    <col min="4" max="4" width="9" style="15" customWidth="1"/>
+    <col min="5" max="5" width="9" style="15" customWidth="1"/>
+    <col min="6" max="6" width="9" style="15" customWidth="1"/>
     <col min="7" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" customHeight="1" ht="15">
       <c r="A1" s="6" t="s">
         <v>353</v>
       </c>
@@ -7433,7 +6958,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" customHeight="1" ht="126">
       <c r="A2" s="16" t="s">
         <v>365</v>
       </c>
@@ -7442,56 +6967,56 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" customHeight="1" ht="15">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" customHeight="1" ht="15">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" customHeight="1" ht="15">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" customHeight="1" ht="15">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" customHeight="1" ht="15">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" customHeight="1" ht="15">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" customHeight="1" ht="15">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" customHeight="1" ht="15">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -7513,7 +7038,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="14.3515625" style="17" customWidth="1"/>
     <col min="2" max="2" width="22.46875" style="17" customWidth="1"/>
@@ -7525,7 +7050,7 @@
     <col min="8" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" customHeight="1" ht="15">
       <c r="A1" s="6" t="s">
         <v>367</v>
       </c>
@@ -7545,7 +7070,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" customHeight="1" ht="15">
       <c r="A2" s="6" t="s">
         <v>373</v>
       </c>
@@ -7565,7 +7090,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" customHeight="1" ht="15">
       <c r="A3" s="6" t="s">
         <v>378</v>
       </c>
@@ -7585,7 +7110,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" customHeight="1" ht="15">
       <c r="A4" s="6" t="s">
         <v>373</v>
       </c>
@@ -7603,7 +7128,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" customHeight="1" ht="15">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -7611,7 +7136,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" customHeight="1" ht="15">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -7619,7 +7144,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" customHeight="1" ht="15">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -7627,7 +7152,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" customHeight="1" ht="15">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -7635,7 +7160,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" customHeight="1" ht="15">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -7643,7 +7168,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" customHeight="1" ht="15">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -7671,16 +7196,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="14" style="18" customWidth="1"/>
     <col min="2" max="2" width="33.17578125" style="18" customWidth="1"/>
     <col min="3" max="3" width="18.17578125" style="18" customWidth="1"/>
-    <col min="4" max="6" width="9" style="18" customWidth="1"/>
+    <col min="4" max="4" width="9" style="18" customWidth="1"/>
+    <col min="5" max="5" width="9" style="18" customWidth="1"/>
+    <col min="6" max="6" width="9" style="18" customWidth="1"/>
     <col min="7" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" customHeight="1" ht="15">
       <c r="A1" s="6" t="s">
         <v>384</v>
       </c>
@@ -7693,7 +7220,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" customHeight="1" ht="15">
       <c r="A2" s="6" t="s">
         <v>387</v>
       </c>
@@ -7706,7 +7233,7 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" customHeight="1" ht="15">
       <c r="A3" s="6" t="s">
         <v>390</v>
       </c>
@@ -7719,7 +7246,7 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" customHeight="1" ht="15">
       <c r="A4" s="6" t="s">
         <v>391</v>
       </c>
@@ -7732,7 +7259,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" customHeight="1" ht="15">
       <c r="A5" s="6" t="s">
         <v>393</v>
       </c>
@@ -7745,35 +7272,35 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" customHeight="1" ht="15">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" customHeight="1" ht="15">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" customHeight="1" ht="15">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" customHeight="1" ht="15">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" customHeight="1" ht="15">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -7795,15 +7322,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="59.46875" style="20" customWidth="1"/>
     <col min="2" max="2" width="43.64453125" style="20" customWidth="1"/>
-    <col min="3" max="6" width="9" style="20" customWidth="1"/>
+    <col min="3" max="3" width="9" style="20" customWidth="1"/>
+    <col min="4" max="4" width="9" style="20" customWidth="1"/>
+    <col min="5" max="5" width="9" style="20" customWidth="1"/>
+    <col min="6" max="6" width="9" style="20" customWidth="1"/>
     <col min="7" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" customHeight="1" ht="15">
       <c r="A1" s="6" t="s">
         <v>395</v>
       </c>
@@ -7816,7 +7346,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
     </row>
-    <row r="2" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" customHeight="1" ht="15">
       <c r="A2" s="6" t="s">
         <v>397</v>
       </c>
@@ -7827,56 +7357,56 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="3" customHeight="1" ht="15">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" customHeight="1" ht="15">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" customHeight="1" ht="15">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" customHeight="1" ht="15">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" customHeight="1" ht="15">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" customHeight="1" ht="15">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" customHeight="1" ht="15">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" customHeight="1" ht="15">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>

</xml_diff>

<commit_message>
shoppingTab method was created
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/ecommerce.xlsx
+++ b/src/main/resources/testData/ecommerce.xlsx
@@ -1321,11 +1321,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="d&quot;-&quot;mm&quot;-&quot;yyyy"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="d&quot;-&quot;mm&quot;-&quot;yyyy"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1392,39 +1392,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1437,10 +1407,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1449,14 +1443,6 @@
       <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1475,16 +1461,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1497,8 +1504,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1506,7 +1514,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1517,14 +1525,6 @@
       <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1555,13 +1555,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1573,13 +1663,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1591,25 +1687,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1621,7 +1705,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1633,67 +1717,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1705,37 +1735,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1809,20 +1809,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1832,6 +1836,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1868,24 +1881,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1894,145 +1894,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2091,7 +2091,7 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3478,7 +3478,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.8" outlineLevelRow="1"/>

</xml_diff>